<commit_message>
- accel calc fixed
</commit_message>
<xml_diff>
--- a/build/acceleration_calc.xlsx
+++ b/build/acceleration_calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elijah/Documents/workspace/GB-Kun/build/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6EC84A-651F-2D4A-9D6F-6BB2C1083B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93247BEF-E33E-3048-B0DE-23512ED5F648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="19620" windowHeight="11360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,9 +29,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Среднее геометрическое:</t>
+  </si>
+  <si>
+    <t>f/s acceleration</t>
+  </si>
+  <si>
+    <t>s/f acceleration</t>
+  </si>
+  <si>
+    <t>P_their</t>
+  </si>
+  <si>
+    <t>P_our</t>
+  </si>
+  <si>
+    <t>T_their</t>
+  </si>
+  <si>
+    <t>T_our</t>
   </si>
 </sst>
 </file>
@@ -383,357 +401,377 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>835.53</v>
-      </c>
-      <c r="B1">
-        <v>507.7</v>
-      </c>
-      <c r="C1">
-        <f>A1/B1</f>
-        <v>1.6457159740003939</v>
-      </c>
-      <c r="F1">
-        <v>835.53</v>
-      </c>
-      <c r="G1">
-        <v>505.74</v>
-      </c>
-      <c r="H1">
-        <f>G1/F1</f>
-        <v>0.60529244910416147</v>
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2094.92</v>
+        <v>835.53</v>
       </c>
       <c r="B2">
-        <v>4278.2</v>
+        <v>507.7</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C21" si="0">A2/B2</f>
-        <v>0.48967322705810856</v>
+        <f>A2/B2</f>
+        <v>1.6457159740003939</v>
       </c>
       <c r="F2">
-        <v>2094.92</v>
+        <v>835.53</v>
       </c>
       <c r="G2">
-        <v>3794.45</v>
+        <v>505.74</v>
       </c>
       <c r="H2">
-        <f>G2/F2</f>
-        <v>1.8112624825769001</v>
+        <f t="shared" ref="H2:H16" si="0">G2/F2</f>
+        <v>0.60529244910416147</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2448.13</v>
+        <v>2094.92</v>
       </c>
       <c r="B3">
-        <v>4394.5200000000004</v>
+        <v>4278.2</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
-        <v>0.55708700836496361</v>
+        <f t="shared" ref="C3:C16" si="1">A3/B3</f>
+        <v>0.48967322705810856</v>
       </c>
       <c r="F3">
-        <v>2448.13</v>
+        <v>2094.92</v>
       </c>
       <c r="G3">
-        <v>4748.33</v>
+        <v>3794.45</v>
       </c>
       <c r="H3">
-        <f>G3/F3</f>
-        <v>1.9395742873131736</v>
+        <f t="shared" si="0"/>
+        <v>1.8112624825769001</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2565.62</v>
+        <v>2448.13</v>
       </c>
       <c r="B4">
-        <v>2817.74</v>
+        <v>4394.5200000000004</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>0.91052403699418683</v>
+        <f t="shared" si="1"/>
+        <v>0.55708700836496361</v>
       </c>
       <c r="F4">
-        <v>2565.62</v>
+        <v>2448.13</v>
       </c>
       <c r="G4">
-        <v>3034.15</v>
+        <v>4748.33</v>
       </c>
       <c r="H4">
-        <f>G4/F4</f>
-        <v>1.1826186262969576</v>
+        <f t="shared" si="0"/>
+        <v>1.9395742873131736</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>3035.77</v>
+        <v>2565.62</v>
       </c>
       <c r="B5">
-        <v>3366.55</v>
+        <v>2817.74</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>0.90174510997905866</v>
+        <f t="shared" si="1"/>
+        <v>0.91052403699418683</v>
       </c>
       <c r="F5">
-        <v>3035.77</v>
+        <v>2565.62</v>
       </c>
       <c r="G5">
-        <v>3545.49</v>
+        <v>3034.15</v>
       </c>
       <c r="H5">
-        <f>G5/F5</f>
-        <v>1.1679046831611091</v>
+        <f t="shared" si="0"/>
+        <v>1.1826186262969576</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2943.96</v>
+        <v>3035.77</v>
       </c>
       <c r="B6">
-        <v>3508.64</v>
+        <v>3366.55</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>0.83906014866158973</v>
+        <f t="shared" si="1"/>
+        <v>0.90174510997905866</v>
       </c>
       <c r="F6">
-        <v>2943.96</v>
+        <v>3035.77</v>
       </c>
       <c r="G6">
-        <v>3045.62</v>
+        <v>3545.49</v>
       </c>
       <c r="H6">
-        <f>G6/F6</f>
-        <v>1.0345317191809671</v>
+        <f t="shared" si="0"/>
+        <v>1.1679046831611091</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1994.27</v>
+        <v>2943.96</v>
       </c>
       <c r="B7">
-        <v>2910.37</v>
+        <v>3508.64</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>0.68522902586269097</v>
+        <f t="shared" si="1"/>
+        <v>0.83906014866158973</v>
       </c>
       <c r="F7">
-        <v>1994.27</v>
+        <v>2943.96</v>
       </c>
       <c r="G7">
-        <v>2953.95</v>
+        <v>3045.62</v>
       </c>
       <c r="H7">
-        <f>G7/F7</f>
-        <v>1.4812186915512944</v>
+        <f t="shared" si="0"/>
+        <v>1.0345317191809671</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>1521</v>
+        <v>1994.27</v>
       </c>
       <c r="B8">
-        <v>1665.49</v>
+        <v>2910.37</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
-        <v>0.91324475079406064</v>
+        <f t="shared" si="1"/>
+        <v>0.68522902586269097</v>
       </c>
       <c r="F8">
-        <v>1521</v>
+        <v>1994.27</v>
       </c>
       <c r="G8">
-        <v>1403.01</v>
+        <v>2953.95</v>
       </c>
       <c r="H8">
-        <f>G8/F8</f>
-        <v>0.92242603550295854</v>
+        <f t="shared" si="0"/>
+        <v>1.4812186915512944</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>3772.7</v>
+        <v>1521</v>
       </c>
       <c r="B9">
-        <v>4348.79</v>
+        <v>1665.49</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
-        <v>0.86752866889410618</v>
+        <f t="shared" si="1"/>
+        <v>0.91324475079406064</v>
       </c>
       <c r="F9">
-        <v>3772.7</v>
+        <v>1521</v>
       </c>
       <c r="G9">
-        <v>3918.84</v>
+        <v>1403.01</v>
       </c>
       <c r="H9">
-        <f>G9/F9</f>
-        <v>1.0387361836350626</v>
+        <f t="shared" si="0"/>
+        <v>0.92242603550295854</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>4609.92</v>
+        <v>3772.7</v>
       </c>
       <c r="B10">
-        <v>5878.65</v>
+        <v>4348.79</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
-        <v>0.78418004133602104</v>
+        <f t="shared" si="1"/>
+        <v>0.86752866889410618</v>
       </c>
       <c r="F10">
-        <v>4609.92</v>
+        <v>3772.7</v>
       </c>
       <c r="G10">
-        <v>5033.2700000000004</v>
+        <v>3918.84</v>
       </c>
       <c r="H10">
-        <f>G10/F10</f>
-        <v>1.0918345654588366</v>
+        <f t="shared" si="0"/>
+        <v>1.0387361836350626</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>3534.93</v>
+        <v>4609.92</v>
       </c>
       <c r="B11">
-        <v>4372.46</v>
+        <v>5878.65</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>0.80845336492500786</v>
+        <f t="shared" si="1"/>
+        <v>0.78418004133602104</v>
       </c>
       <c r="F11">
-        <v>3534.93</v>
+        <v>4609.92</v>
       </c>
       <c r="G11">
-        <v>3158.89</v>
+        <v>5033.2700000000004</v>
       </c>
       <c r="H11">
-        <f>G11/F11</f>
-        <v>0.89362165587437381</v>
+        <f t="shared" si="0"/>
+        <v>1.0918345654588366</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>3764.26</v>
+        <v>3534.93</v>
       </c>
       <c r="B12">
-        <v>5442.59</v>
+        <v>4372.46</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
-        <v>0.69163027161700585</v>
+        <f t="shared" si="1"/>
+        <v>0.80845336492500786</v>
       </c>
       <c r="F12">
-        <v>3764.26</v>
+        <v>3534.93</v>
       </c>
       <c r="G12">
-        <v>5882.75</v>
+        <v>3158.89</v>
       </c>
       <c r="H12">
-        <f>G12/F12</f>
-        <v>1.562790561757158</v>
+        <f t="shared" si="0"/>
+        <v>0.89362165587437381</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>533.53</v>
+        <v>3764.26</v>
       </c>
       <c r="B13">
-        <v>2593.66</v>
+        <v>5442.59</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
-        <v>0.2057054509843233</v>
+        <f t="shared" si="1"/>
+        <v>0.69163027161700585</v>
       </c>
       <c r="F13">
-        <v>533.53</v>
+        <v>3764.26</v>
       </c>
       <c r="G13">
-        <v>1904.85</v>
+        <v>5882.75</v>
       </c>
       <c r="H13">
-        <f>G13/F13</f>
-        <v>3.5702772102787099</v>
+        <f t="shared" si="0"/>
+        <v>1.562790561757158</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>1422.59</v>
+        <v>533.53</v>
       </c>
       <c r="B14">
-        <v>2080.52</v>
+        <v>2593.66</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
-        <v>0.68376655836040989</v>
+        <f t="shared" si="1"/>
+        <v>0.2057054509843233</v>
       </c>
       <c r="F14">
-        <v>1422.59</v>
+        <v>533.53</v>
       </c>
       <c r="G14">
-        <v>2552</v>
+        <v>1904.85</v>
       </c>
       <c r="H14">
-        <f>G14/F14</f>
-        <v>1.7939111057999846</v>
+        <f t="shared" si="0"/>
+        <v>3.5702772102787099</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
+        <v>1422.59</v>
+      </c>
+      <c r="B15">
+        <v>2080.52</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>0.68376655836040989</v>
+      </c>
+      <c r="F15">
+        <v>1422.59</v>
+      </c>
+      <c r="G15">
+        <v>2552</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>1.7939111057999846</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>5561.02</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>6828.63</v>
       </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
+      <c r="C16">
+        <f t="shared" si="1"/>
         <v>0.81436832863985897</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>5561.02</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <v>5080.9799999999996</v>
       </c>
-      <c r="H15">
-        <f>G15/F15</f>
+      <c r="H16">
+        <f t="shared" si="0"/>
         <v>0.91367770660778047</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>0</v>
       </c>
-      <c r="D25">
-        <f>GEOMEAN(C4:C24)</f>
+      <c r="D26">
+        <f>GEOMEAN(C5:C25)</f>
         <v>0.71804147441730892</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F26" t="s">
         <v>0</v>
       </c>
-      <c r="I25">
-        <f>GEOMEAN(H1:H23)</f>
+      <c r="I26">
+        <f>GEOMEAN(H2:H24)</f>
         <v>1.2755010244256137</v>
       </c>
     </row>

</xml_diff>